<commit_message>
added variant files + output folder
</commit_message>
<xml_diff>
--- a/report/input/pws_other.xlsx
+++ b/report/input/pws_other.xlsx
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1053,7 +1053,7 @@
         <v>78</v>
       </c>
       <c r="K11" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1884,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="N25" t="n">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="O25" t="n">
         <v>0</v>
@@ -3075,10 +3075,10 @@
         <v>413</v>
       </c>
       <c r="G45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I45" t="n">
         <v>11</v>
@@ -3087,7 +3087,7 @@
         <v>8996</v>
       </c>
       <c r="K45" t="n">
-        <v>9408</v>
+        <v>9409</v>
       </c>
       <c r="L45" t="n">
         <v>0</v>
@@ -3096,7 +3096,7 @@
         <v>0</v>
       </c>
       <c r="N45" t="n">
-        <v>9414</v>
+        <v>9409</v>
       </c>
       <c r="O45" t="n">
         <v>0</v>
@@ -4155,10 +4155,10 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" t="n">
         <v>0</v>
@@ -4176,7 +4176,7 @@
         <v>0</v>
       </c>
       <c r="N63" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O63" t="n">
         <v>0</v>
@@ -5349,10 +5349,10 @@
         <v>309</v>
       </c>
       <c r="G83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" t="n">
         <v>549</v>
@@ -5370,7 +5370,7 @@
         <v>0</v>
       </c>
       <c r="N83" t="n">
-        <v>26309</v>
+        <v>26308</v>
       </c>
       <c r="O83" t="n">
         <v>0</v>
@@ -6429,10 +6429,10 @@
         <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101" t="n">
         <v>0</v>
@@ -6450,7 +6450,7 @@
         <v>0</v>
       </c>
       <c r="N101" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O101" t="n">
         <v>0</v>
@@ -7623,10 +7623,10 @@
         <v>33</v>
       </c>
       <c r="G121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121" t="n">
         <v>0</v>
@@ -7644,7 +7644,7 @@
         <v>0</v>
       </c>
       <c r="N121" t="n">
-        <v>5335</v>
+        <v>5334</v>
       </c>
       <c r="O121" t="n">
         <v>0</v>
@@ -13251,10 +13251,10 @@
         <v>0</v>
       </c>
       <c r="G215" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H215" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I215" t="n">
         <v>0</v>
@@ -13272,7 +13272,7 @@
         <v>0</v>
       </c>
       <c r="N215" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O215" t="n">
         <v>0</v>
@@ -14445,10 +14445,10 @@
         <v>277</v>
       </c>
       <c r="G235" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H235" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I235" t="n">
         <v>133</v>
@@ -14466,7 +14466,7 @@
         <v>0</v>
       </c>
       <c r="N235" t="n">
-        <v>19887</v>
+        <v>19886</v>
       </c>
       <c r="O235" t="n">
         <v>0</v>
@@ -15525,7 +15525,7 @@
         <v>4</v>
       </c>
       <c r="G253" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H253" t="n">
         <v>0</v>
@@ -15534,11 +15534,11 @@
         <v>0</v>
       </c>
       <c r="J253" t="n">
+        <v>212</v>
+      </c>
+      <c r="K253" t="n">
         <v>216</v>
       </c>
-      <c r="K253" t="n">
-        <v>220</v>
-      </c>
       <c r="L253" t="n">
         <v>0</v>
       </c>
@@ -15546,7 +15546,7 @@
         <v>0</v>
       </c>
       <c r="N253" t="n">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="O253" t="n">
         <v>0</v>
@@ -15558,7 +15558,7 @@
         <v>4</v>
       </c>
       <c r="R253" t="n">
-        <v>1382</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="254">
@@ -16719,7 +16719,7 @@
         <v>7916</v>
       </c>
       <c r="G273" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H273" t="n">
         <v>0</v>
@@ -16728,10 +16728,10 @@
         <v>1368</v>
       </c>
       <c r="J273" t="n">
-        <v>13751</v>
+        <v>13747</v>
       </c>
       <c r="K273" t="n">
-        <v>21667</v>
+        <v>21663</v>
       </c>
       <c r="L273" t="n">
         <v>0</v>
@@ -16740,7 +16740,7 @@
         <v>0</v>
       </c>
       <c r="N273" t="n">
-        <v>21667</v>
+        <v>21663</v>
       </c>
       <c r="O273" t="n">
         <v>0</v>
@@ -16752,7 +16752,7 @@
         <v>144</v>
       </c>
       <c r="R273" t="n">
-        <v>41965</v>
+        <v>41969</v>
       </c>
     </row>
     <row r="274">
@@ -53886,7 +53886,7 @@
         <v>0</v>
       </c>
       <c r="H894" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="I894" t="n">
         <v>0</v>
@@ -53904,7 +53904,7 @@
         <v>0</v>
       </c>
       <c r="N894" t="n">
-        <v>594</v>
+        <v>552</v>
       </c>
       <c r="O894" t="n">
         <v>0</v>
@@ -55500,7 +55500,7 @@
         <v>0</v>
       </c>
       <c r="H921" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="I921" t="n">
         <v>25</v>
@@ -55518,7 +55518,7 @@
         <v>0</v>
       </c>
       <c r="N921" t="n">
-        <v>16321</v>
+        <v>16279</v>
       </c>
       <c r="O921" t="n">
         <v>0</v>
@@ -65673,10 +65673,10 @@
         <v>0</v>
       </c>
       <c r="G1091" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H1091" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I1091" t="n">
         <v>0</v>
@@ -65685,7 +65685,7 @@
         <v>8</v>
       </c>
       <c r="K1091" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L1091" t="n">
         <v>0</v>
@@ -65694,7 +65694,7 @@
         <v>0</v>
       </c>
       <c r="N1091" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O1091" t="n">
         <v>0</v>
@@ -66867,10 +66867,10 @@
         <v>0</v>
       </c>
       <c r="G1111" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H1111" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I1111" t="n">
         <v>0</v>
@@ -66879,7 +66879,7 @@
         <v>21</v>
       </c>
       <c r="K1111" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="L1111" t="n">
         <v>0</v>
@@ -66888,7 +66888,7 @@
         <v>0</v>
       </c>
       <c r="N1111" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="O1111" t="n">
         <v>0</v>
@@ -77558,10 +77558,10 @@
         <v>0</v>
       </c>
       <c r="J1285" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K1285" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L1285" t="n">
         <v>0</v>
@@ -77570,7 +77570,7 @@
         <v>0</v>
       </c>
       <c r="N1285" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O1285" t="n">
         <v>0</v>
@@ -77682,10 +77682,10 @@
         <v>0</v>
       </c>
       <c r="J1287" t="n">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="K1287" t="n">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="L1287" t="n">
         <v>0</v>
@@ -77694,7 +77694,7 @@
         <v>0</v>
       </c>
       <c r="N1287" t="n">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="O1287" t="n">
         <v>0</v>
@@ -78542,10 +78542,10 @@
         <v>0</v>
       </c>
       <c r="J1301" t="n">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="K1301" t="n">
-        <v>2127</v>
+        <v>2125</v>
       </c>
       <c r="L1301" t="n">
         <v>0</v>
@@ -78554,7 +78554,7 @@
         <v>0</v>
       </c>
       <c r="N1301" t="n">
-        <v>2127</v>
+        <v>2125</v>
       </c>
       <c r="O1301" t="n">
         <v>0</v>
@@ -79218,7 +79218,7 @@
         <v>0</v>
       </c>
       <c r="H1312" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I1312" t="n">
         <v>100</v>
@@ -79236,7 +79236,7 @@
         <v>0</v>
       </c>
       <c r="N1312" t="n">
-        <v>593</v>
+        <v>533</v>
       </c>
       <c r="O1312" t="n">
         <v>0</v>
@@ -80884,7 +80884,7 @@
         <v>0</v>
       </c>
       <c r="H1339" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I1339" t="n">
         <v>252</v>
@@ -80902,7 +80902,7 @@
         <v>0</v>
       </c>
       <c r="N1339" t="n">
-        <v>2835</v>
+        <v>2775</v>
       </c>
       <c r="O1339" t="n">
         <v>0</v>

</xml_diff>